<commit_message>
[FIX] add fields reference in withholding tax report
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_withholding_income_tax.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_withholding_income_tax.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">ใบแนบ</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t xml:space="preserve">เลขที่เอกสาร</t>
+  </si>
+  <si>
+    <t xml:space="preserve">อ้างอิง</t>
   </si>
 </sst>
 </file>
@@ -294,7 +297,7 @@
   <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,7 +387,9 @@
       <c r="K5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="13"/>
+      <c r="L5" s="11" t="s">
+        <v>15</v>
+      </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>

</xml_diff>

<commit_message>
[FIX] switch column withholding_tax excel
</commit_message>
<xml_diff>
--- a/cmo_account_report/xlsx_template/xlsx_report_withholding_income_tax.xlsx
+++ b/cmo_account_report/xlsx_template/xlsx_report_withholding_income_tax.xlsx
@@ -37,6 +37,9 @@
     <t xml:space="preserve">ลำดับที่</t>
   </si>
   <si>
+    <t xml:space="preserve">เลขที่เอกสาร</t>
+  </si>
+  <si>
     <t xml:space="preserve">เลขประจำตัวผู้เสียภาษีอากร</t>
   </si>
   <si>
@@ -62,9 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve">เงื่อนไขการชำระเงิน</t>
-  </si>
-  <si>
-    <t xml:space="preserve">เลขที่เอกสาร</t>
   </si>
   <si>
     <t xml:space="preserve">อ้างอิง</t>
@@ -294,7 +294,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:AMJ5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -303,16 +303,17 @@
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="36.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.9"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.61"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="3" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.75"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="36.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.9"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="8.61"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="3" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -327,31 +328,37 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="C2" s="6"/>
+      <c r="H2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="6"/>
-      <c r="G3" s="8"/>
-      <c r="J3" s="9" t="s">
+      <c r="C3" s="6"/>
+      <c r="H3" s="8"/>
+      <c r="K3" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="14" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
@@ -372,10 +379,10 @@
       <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="11" t="s">
@@ -403,13 +410,14 @@
       <c r="W5" s="13"/>
       <c r="X5" s="13"/>
       <c r="Y5" s="13"/>
+      <c r="AMJ5" s="0"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="A3:C3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>